<commit_message>
data from forward renderer and fixed some potential bugs
</commit_message>
<xml_diff>
--- a/documents/data/test_data.xlsx
+++ b/documents/data/test_data.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="29">
   <si>
     <t>Sponza 1000 large lights (10.0f)</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>Sponza 200 lights (5.0f)</t>
+  </si>
+  <si>
+    <t>Crashed Computer</t>
+  </si>
+  <si>
+    <t>N/A</t>
   </si>
 </sst>
 </file>
@@ -458,8 +464,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -500,8 +506,14 @@
       <c r="B4">
         <v>2.71</v>
       </c>
+      <c r="C4">
+        <v>5.98</v>
+      </c>
       <c r="D4">
         <v>369</v>
+      </c>
+      <c r="E4">
+        <v>167.22</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -511,8 +523,14 @@
       <c r="B5">
         <v>5.97</v>
       </c>
+      <c r="C5">
+        <v>55.95</v>
+      </c>
       <c r="D5">
         <v>167.5</v>
+      </c>
+      <c r="E5">
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -522,8 +540,14 @@
       <c r="B6">
         <v>4.91</v>
       </c>
+      <c r="C6">
+        <v>264.82</v>
+      </c>
       <c r="D6">
         <v>203.66</v>
+      </c>
+      <c r="E6">
+        <v>3.78</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -533,8 +557,14 @@
       <c r="B7">
         <v>21.98</v>
       </c>
+      <c r="C7">
+        <v>268.26</v>
+      </c>
       <c r="D7">
         <v>45.5</v>
+      </c>
+      <c r="E7">
+        <v>3.73</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -542,10 +572,16 @@
         <v>0</v>
       </c>
       <c r="B8">
-        <v>174.03</v>
+        <v>73.23</v>
+      </c>
+      <c r="C8">
+        <v>293.08999999999997</v>
       </c>
       <c r="D8">
-        <v>5.75</v>
+        <v>13.66</v>
+      </c>
+      <c r="E8">
+        <v>3.41</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -555,8 +591,14 @@
       <c r="B9">
         <v>54.83</v>
       </c>
+      <c r="C9" t="s">
+        <v>27</v>
+      </c>
       <c r="D9">
         <v>18.23</v>
+      </c>
+      <c r="E9" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -566,8 +608,14 @@
       <c r="B10">
         <v>9.9</v>
       </c>
+      <c r="C10">
+        <v>8.7200000000000006</v>
+      </c>
       <c r="D10">
         <v>101.01</v>
+      </c>
+      <c r="E10">
+        <v>114.68</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -577,8 +625,14 @@
       <c r="B11">
         <v>11.82</v>
       </c>
+      <c r="C11">
+        <v>122.43</v>
+      </c>
       <c r="D11">
         <v>84.6</v>
+      </c>
+      <c r="E11">
+        <v>32.67</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -588,8 +642,14 @@
       <c r="B12">
         <v>24.59</v>
       </c>
+      <c r="C12">
+        <v>641.05999999999995</v>
+      </c>
       <c r="D12">
         <v>40.67</v>
+      </c>
+      <c r="E12">
+        <v>1.56</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -599,8 +659,14 @@
       <c r="B13">
         <v>345.82</v>
       </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
       <c r="D13">
         <v>2.89</v>
+      </c>
+      <c r="E13" t="s">
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>